<commit_message>
actualizacion de project PC3
</commit_message>
<xml_diff>
--- a/Area de proceso PPQA/Herramienta de aseguramiento de calidad/HGQA_V2.0_2017.xlsx
+++ b/Area de proceso PPQA/Herramienta de aseguramiento de calidad/HGQA_V2.0_2017.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+  <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Desktop/documentationStaradmin/Area de proceso PPQA/Herramienta de aseguramiento de calidad/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="642" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="20500" windowHeight="7760" tabRatio="642" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="14" r:id="rId1"/>
@@ -52,7 +57,15 @@
     <definedName name="TipoServicio" localSheetId="0">#REF!</definedName>
     <definedName name="TiposNC">Tablas!$F$3:$F$8</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -894,7 +907,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
   </numFmts>
-  <fonts count="60">
+  <fonts count="60" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1520,107 +1533,107 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1628,10 +1641,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1639,23 +1652,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1663,96 +1676,96 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1760,7 +1773,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1768,58 +1781,58 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1827,23 +1840,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1851,56 +1864,56 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1908,14 +1921,14 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2446,6 +2459,10 @@
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="43" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2455,14 +2472,35 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2515,30 +2553,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2548,26 +2581,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="34" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2580,6 +2593,34 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="56" fillId="25" borderId="10" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2591,18 +2632,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="33" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -2628,22 +2657,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2679,7 +2692,7 @@
     <cellStyle name="60% - Énfasis4" xfId="16" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="17" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="19" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="19" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="20" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cancel" xfId="21"/>
     <cellStyle name="Celda de comprobación" xfId="22" builtinId="23" customBuiltin="1"/>
@@ -2769,8 +2782,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.30687900123595707"/>
-          <c:y val="4.4982698961937774E-2"/>
+          <c:x val="0.306879001235957"/>
+          <c:y val="0.0449826989619378"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2803,10 +2816,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.29638041791176717"/>
-          <c:y val="0.35682819383259951"/>
-          <c:w val="0.40724026888639714"/>
-          <c:h val="0.31718061674008841"/>
+          <c:x val="0.296380417911767"/>
+          <c:y val="0.3568281938326"/>
+          <c:w val="0.407240268886397"/>
+          <c:h val="0.317180616740088"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -2862,7 +2875,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-ES_tradnl"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -2873,9 +2886,7 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2899,10 +2910,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2931,10 +2942,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1153847428511459"/>
-          <c:y val="0.79295154185021988"/>
-          <c:w val="0.7986434162049908"/>
-          <c:h val="9.6916299559471397E-2"/>
+          <c:x val="0.115384742851146"/>
+          <c:y val="0.79295154185022"/>
+          <c:w val="0.798643416204991"/>
+          <c:h val="0.0969162995594714"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2963,7 +2974,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2996,12 +3007,12 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0" footer="0"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.0" footer="0.0"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3048,8 +3059,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.28496549382376185"/>
-          <c:y val="5.4727021062665721E-2"/>
+          <c:x val="0.284965493823762"/>
+          <c:y val="0.0547270210626657"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3082,10 +3093,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39860190899433157"/>
-          <c:y val="0.39303816764222554"/>
-          <c:w val="0.20279746247080033"/>
-          <c:h val="0.22885766723471332"/>
+          <c:x val="0.398601908994332"/>
+          <c:y val="0.393038167642226"/>
+          <c:w val="0.2027974624708"/>
+          <c:h val="0.228857667234713"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -3180,8 +3191,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.8328551530876594E-3"/>
-                  <c:y val="3.9269553691714185E-2"/>
+                  <c:x val="-0.00683285515308766"/>
+                  <c:y val="0.0392695536917142"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -3192,17 +3203,15 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.0718556028495433E-2"/>
-                  <c:y val="1.9369539879113832E-2"/>
+                  <c:x val="0.0307185560284954"/>
+                  <c:y val="0.0193695398791138"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -3213,17 +3222,15 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="7.5132877704156803E-2"/>
-                  <c:y val="-9.9676402646107332E-2"/>
+                  <c:x val="0.0751328777041568"/>
+                  <c:y val="-0.0996764026461073"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="bestFit"/>
@@ -3234,9 +3241,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -3260,7 +3265,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-ES_tradnl"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="1"/>
@@ -3271,9 +3276,7 @@
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3306,19 +3309,19 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3347,10 +3350,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="2.4663677130044841E-2"/>
-          <c:y val="0.83974884658482774"/>
-          <c:w val="0.94843049327354301"/>
-          <c:h val="0.12820593077630954"/>
+          <c:x val="0.0246636771300448"/>
+          <c:y val="0.839748846584828"/>
+          <c:w val="0.948430493273543"/>
+          <c:h val="0.12820593077631"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3379,7 +3382,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3412,12 +3415,12 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0" footer="0"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.0" footer="0.0"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3464,8 +3467,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.28321724207550975"/>
-          <c:y val="4.0498851195002496E-2"/>
+          <c:x val="0.28321724207551"/>
+          <c:y val="0.0404988511950025"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3483,10 +3486,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="8.5664445354045105E-2"/>
-          <c:y val="0.21183913404912819"/>
-          <c:w val="0.88112000935589063"/>
-          <c:h val="0.58878818140125222"/>
+          <c:x val="0.0856644453540451"/>
+          <c:y val="0.211839134049128"/>
+          <c:w val="0.881120009355891"/>
+          <c:h val="0.588788181401252"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3594,7 +3597,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-ES_tradnl"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -3607,7 +3610,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3651,11 +3653,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="169686144"/>
-        <c:axId val="169689472"/>
+        <c:axId val="-1364318816"/>
+        <c:axId val="-1364317040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="169686144"/>
+        <c:axId val="-1364318816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3687,10 +3689,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169689472"/>
+        <c:crossAx val="-1364317040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3700,7 +3702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169689472"/>
+        <c:axId val="-1364317040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3742,10 +3744,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169686144"/>
+        <c:crossAx val="-1364318816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3767,10 +3769,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.2017937219730942"/>
-          <c:y val="0.82800161719065901"/>
-          <c:w val="0.63004484304932784"/>
-          <c:h val="6.4000125000244143E-2"/>
+          <c:x val="0.201793721973094"/>
+          <c:y val="0.828001617190659"/>
+          <c:w val="0.630044843049328"/>
+          <c:h val="0.0640001250002441"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3799,7 +3801,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3832,12 +3834,12 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3884,8 +3886,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.34622144112478037"/>
-          <c:y val="4.4776609080581398E-2"/>
+          <c:x val="0.34622144112478"/>
+          <c:y val="0.0447766090805814"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3952,10 +3954,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.12829525483304044"/>
-          <c:y val="0.18656826890973721"/>
-          <c:w val="0.63796133567662561"/>
-          <c:h val="0.6119439220239381"/>
+          <c:x val="0.12829525483304"/>
+          <c:y val="0.186568268909737"/>
+          <c:w val="0.637961335676626"/>
+          <c:h val="0.611943922023938"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
@@ -4009,7 +4011,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-ES_tradnl"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4021,7 +4023,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4033,7 +4034,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4086,7 +4087,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-ES_tradnl"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4098,7 +4099,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4110,7 +4110,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4163,7 +4163,7 @@
                     <a:cs typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-ES_tradnl"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -4175,7 +4175,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -4187,7 +4186,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4203,12 +4202,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="169952000"/>
-        <c:axId val="169953920"/>
+        <c:axId val="-1399703328"/>
+        <c:axId val="-1399699472"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="169952000"/>
+        <c:axId val="-1399703328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4241,8 +4240,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.3743409490333921"/>
-              <c:y val="0.86194519528342584"/>
+              <c:x val="0.374340949033392"/>
+              <c:y val="0.861945195283426"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4279,10 +4278,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169953920"/>
+        <c:crossAx val="-1399699472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4292,7 +4291,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="169953920"/>
+        <c:axId val="-1399699472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4335,8 +4334,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="7.9086115992970163E-2"/>
-              <c:y val="0.53358502761781645"/>
+              <c:x val="0.0790861159929702"/>
+              <c:y val="0.533585027617816"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4373,10 +4372,10 @@
                 <a:cs typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="169952000"/>
+        <c:crossAx val="-1399703328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4393,10 +4392,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78603776489865906"/>
-          <c:y val="0.48803827751196188"/>
-          <c:w val="0.19819863412917491"/>
-          <c:h val="0.15311004784689006"/>
+          <c:x val="0.786037764898659"/>
+          <c:y val="0.488038277511962"/>
+          <c:w val="0.198198634129175"/>
+          <c:h val="0.15311004784689"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4425,7 +4424,7 @@
               <a:cs typeface="Arial"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-ES_tradnl"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4458,12 +4457,12 @@
           <a:cs typeface="Arial"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-ES_tradnl"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0" footer="0"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.0" footer="0.0"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4838,12 +4837,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -4873,12 +4872,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -5082,27 +5081,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="66" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="66" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="66" customWidth="1"/>
     <col min="3" max="3" width="9" style="66" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="66" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="66" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="66" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="66" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="66" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="66" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" style="66" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="66" customWidth="1"/>
     <col min="8" max="8" width="15" style="66" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="66"/>
+    <col min="9" max="16384" width="9.1640625" style="66"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="65"/>
       <c r="B1" s="65"/>
       <c r="C1" s="65"/>
@@ -5113,7 +5112,7 @@
       <c r="H1" s="65"/>
       <c r="I1" s="65"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75">
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="65"/>
       <c r="B2" s="149" t="s">
         <v>62</v>
@@ -5126,7 +5125,7 @@
       <c r="H2" s="149"/>
       <c r="I2" s="65"/>
     </row>
-    <row r="3" spans="1:9" ht="13.5" thickBot="1">
+    <row r="3" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="65"/>
       <c r="B3" s="65"/>
       <c r="C3" s="65"/>
@@ -5137,7 +5136,7 @@
       <c r="H3" s="65"/>
       <c r="I3" s="65"/>
     </row>
-    <row r="4" spans="1:9" ht="36.75" customHeight="1" thickBot="1">
+    <row r="4" spans="1:9" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="65"/>
       <c r="B4" s="67" t="s">
         <v>63</v>
@@ -5162,7 +5161,7 @@
       </c>
       <c r="I4" s="65"/>
     </row>
-    <row r="5" spans="1:9" ht="24">
+    <row r="5" spans="1:9" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="65"/>
       <c r="B5" s="70">
         <v>1</v>
@@ -5187,7 +5186,7 @@
       </c>
       <c r="I5" s="65"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="65"/>
       <c r="B6" s="76"/>
       <c r="C6" s="129"/>
@@ -5198,7 +5197,7 @@
       <c r="H6" s="80"/>
       <c r="I6" s="65"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="65"/>
       <c r="B7" s="76"/>
       <c r="C7" s="130"/>
@@ -5209,7 +5208,7 @@
       <c r="H7" s="83"/>
       <c r="I7" s="65"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="65"/>
       <c r="B8" s="70"/>
       <c r="C8" s="71"/>
@@ -5220,7 +5219,7 @@
       <c r="H8" s="75"/>
       <c r="I8" s="65"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="65"/>
       <c r="B9" s="76"/>
       <c r="C9" s="134"/>
@@ -5231,7 +5230,7 @@
       <c r="H9" s="80"/>
       <c r="I9" s="65"/>
     </row>
-    <row r="10" spans="1:9" ht="13.5" thickBot="1">
+    <row r="10" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B10" s="84"/>
       <c r="C10" s="85"/>
       <c r="D10" s="128"/>
@@ -5253,45 +5252,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3" style="38" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="38" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" style="38" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="38"/>
+    <col min="2" max="2" width="27.83203125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="38" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="38" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" style="38" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="61" customFormat="1" ht="12" customHeight="1"/>
-    <row r="2" spans="1:8" s="61" customFormat="1" ht="48.75" customHeight="1">
+    <row r="1" spans="1:8" s="61" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="1:8" s="61" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="39"/>
       <c r="B2" s="62"/>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="170" t="s">
         <v>202</v>
       </c>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
-    </row>
-    <row r="3" spans="1:8" s="61" customFormat="1">
+      <c r="D2" s="171"/>
+      <c r="E2" s="172"/>
+    </row>
+    <row r="3" spans="1:8" s="61" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="39"/>
       <c r="B3" s="148" t="s">
         <v>225</v>
       </c>
-      <c r="C3" s="170" t="s">
+      <c r="C3" s="178" t="s">
         <v>203</v>
       </c>
-      <c r="D3" s="171"/>
-      <c r="E3" s="172"/>
-    </row>
-    <row r="4" spans="1:8" s="61" customFormat="1" ht="21.75" customHeight="1">
+      <c r="D3" s="179"/>
+      <c r="E3" s="180"/>
+    </row>
+    <row r="4" spans="1:8" s="61" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="39"/>
       <c r="B4" s="63" t="s">
         <v>43</v>
@@ -5299,23 +5298,23 @@
       <c r="C4" s="64"/>
       <c r="D4" s="64"/>
     </row>
-    <row r="5" spans="1:8" ht="24.75" customHeight="1">
+    <row r="5" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="39"/>
-      <c r="B5" s="165" t="s">
+      <c r="B5" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="166"/>
-      <c r="D5" s="166"/>
-      <c r="E5" s="167"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="C5" s="174"/>
+      <c r="D5" s="174"/>
+      <c r="E5" s="175"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="39"/>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
       <c r="E6" s="51"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="39"/>
       <c r="B7" s="50" t="s">
         <v>5</v>
@@ -5323,25 +5322,25 @@
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="39"/>
       <c r="B8" s="40" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="90"/>
-      <c r="D8" s="168" t="s">
+      <c r="D8" s="176" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="169"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="E8" s="177"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="39"/>
       <c r="B9" s="91"/>
       <c r="C9" s="64"/>
       <c r="D9" s="92"/>
       <c r="E9" s="92"/>
     </row>
-    <row r="10" spans="1:8" ht="12" customHeight="1">
+    <row r="10" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="39"/>
       <c r="B10" s="93" t="s">
         <v>93</v>
@@ -5352,14 +5351,14 @@
       </c>
       <c r="E10" s="94"/>
     </row>
-    <row r="11" spans="1:8" ht="9.9499999999999993" customHeight="1">
+    <row r="11" spans="1:8" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="39"/>
       <c r="B11" s="95"/>
       <c r="C11" s="61"/>
       <c r="D11" s="96"/>
       <c r="E11" s="96"/>
     </row>
-    <row r="12" spans="1:8" ht="12" customHeight="1">
+    <row r="12" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="39"/>
       <c r="B12" s="97" t="s">
         <v>93</v>
@@ -5370,14 +5369,14 @@
       </c>
       <c r="E12" s="94"/>
     </row>
-    <row r="13" spans="1:8" ht="9.9499999999999993" customHeight="1">
+    <row r="13" spans="1:8" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="39"/>
       <c r="B13" s="61"/>
       <c r="C13" s="61"/>
       <c r="D13" s="96"/>
       <c r="E13" s="96"/>
     </row>
-    <row r="14" spans="1:8" ht="12" customHeight="1">
+    <row r="14" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="37"/>
       <c r="B14" s="98" t="s">
         <v>93</v>
@@ -5388,14 +5387,14 @@
       </c>
       <c r="E14" s="94"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="37"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
       <c r="D15" s="96"/>
       <c r="E15" s="96"/>
     </row>
-    <row r="16" spans="1:8" ht="12" customHeight="1">
+    <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="37"/>
       <c r="B16" s="99" t="s">
         <v>93</v>
@@ -5407,340 +5406,340 @@
       <c r="E16" s="94"/>
       <c r="H16" s="41"/>
     </row>
-    <row r="17" spans="1:8" s="52" customFormat="1" ht="12" customHeight="1">
+    <row r="17" spans="1:8" s="52" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="42"/>
       <c r="B17" s="43"/>
       <c r="D17" s="53"/>
       <c r="E17" s="53"/>
       <c r="H17" s="44"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="37"/>
     </row>
-    <row r="19" spans="1:8" s="57" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B19" s="156" t="s">
+    <row r="19" spans="1:8" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="164" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="157"/>
-      <c r="D19" s="157"/>
-      <c r="E19" s="158"/>
-    </row>
-    <row r="20" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1">
+      <c r="C19" s="165"/>
+      <c r="D19" s="165"/>
+      <c r="E19" s="166"/>
+    </row>
+    <row r="20" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="159" t="s">
+      <c r="C20" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="160"/>
-      <c r="E20" s="161"/>
-    </row>
-    <row r="21" spans="1:8" s="57" customFormat="1" ht="12.75" customHeight="1">
+      <c r="D20" s="168"/>
+      <c r="E20" s="169"/>
+    </row>
+    <row r="21" spans="1:8" s="57" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="173" t="s">
+      <c r="C21" s="155" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="174"/>
-      <c r="E21" s="175"/>
-    </row>
-    <row r="22" spans="1:8" s="57" customFormat="1" ht="12.75" customHeight="1">
+      <c r="D21" s="156"/>
+      <c r="E21" s="157"/>
+    </row>
+    <row r="22" spans="1:8" s="57" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="173" t="s">
+      <c r="C22" s="155" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="174"/>
-      <c r="E22" s="175"/>
-    </row>
-    <row r="23" spans="1:8" s="57" customFormat="1" ht="12.75" customHeight="1">
+      <c r="D22" s="156"/>
+      <c r="E22" s="157"/>
+    </row>
+    <row r="23" spans="1:8" s="57" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="173" t="s">
+      <c r="C23" s="155" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="174"/>
-      <c r="E23" s="175"/>
-    </row>
-    <row r="24" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1">
+      <c r="D23" s="156"/>
+      <c r="E23" s="157"/>
+    </row>
+    <row r="24" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="173" t="s">
+      <c r="C24" s="155" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="174"/>
-      <c r="E24" s="175"/>
-    </row>
-    <row r="25" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1">
+      <c r="D24" s="156"/>
+      <c r="E24" s="157"/>
+    </row>
+    <row r="25" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="59"/>
       <c r="C25" s="60"/>
       <c r="D25" s="60"/>
       <c r="E25" s="60"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="37"/>
       <c r="B26" s="50"/>
     </row>
-    <row r="27" spans="1:8" s="57" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B27" s="156" t="s">
+    <row r="27" spans="1:8" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="164" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="158"/>
-    </row>
-    <row r="28" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1">
+      <c r="C27" s="165"/>
+      <c r="D27" s="165"/>
+      <c r="E27" s="166"/>
+    </row>
+    <row r="28" spans="1:8" s="57" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="159" t="s">
+      <c r="C28" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="160"/>
-      <c r="E28" s="161"/>
-    </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1">
+      <c r="D28" s="168"/>
+      <c r="E28" s="169"/>
+    </row>
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="37"/>
-      <c r="B29" s="176" t="s">
+      <c r="B29" s="161" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="177"/>
-      <c r="D29" s="177"/>
-      <c r="E29" s="178"/>
+      <c r="C29" s="162"/>
+      <c r="D29" s="162"/>
+      <c r="E29" s="163"/>
       <c r="F29" s="57"/>
       <c r="G29" s="57"/>
     </row>
-    <row r="30" spans="1:8" ht="16.5" customHeight="1">
+    <row r="30" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="37"/>
       <c r="B30" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="C30" s="150" t="s">
+      <c r="C30" s="151" t="s">
         <v>166</v>
       </c>
-      <c r="D30" s="151"/>
-      <c r="E30" s="152"/>
+      <c r="D30" s="152"/>
+      <c r="E30" s="153"/>
       <c r="F30" s="57"/>
       <c r="G30" s="57"/>
     </row>
-    <row r="31" spans="1:8" ht="16.5" customHeight="1">
+    <row r="31" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="37"/>
       <c r="B31" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="C31" s="150" t="s">
+      <c r="C31" s="151" t="s">
         <v>168</v>
       </c>
-      <c r="D31" s="151"/>
-      <c r="E31" s="152"/>
+      <c r="D31" s="152"/>
+      <c r="E31" s="153"/>
       <c r="F31" s="57"/>
       <c r="G31" s="57"/>
     </row>
-    <row r="32" spans="1:8" ht="16.5" customHeight="1">
+    <row r="32" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="37"/>
       <c r="B32" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="150" t="s">
+      <c r="C32" s="151" t="s">
         <v>189</v>
       </c>
-      <c r="D32" s="151"/>
-      <c r="E32" s="152"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="153"/>
       <c r="F32" s="57"/>
       <c r="G32" s="57"/>
     </row>
-    <row r="33" spans="1:7" ht="16.5" customHeight="1">
+    <row r="33" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="37"/>
       <c r="B33" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="150" t="s">
+      <c r="C33" s="151" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="151"/>
-      <c r="E33" s="152"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="153"/>
       <c r="F33" s="57"/>
       <c r="G33" s="57"/>
     </row>
-    <row r="34" spans="1:7" ht="16.5" customHeight="1">
+    <row r="34" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="37"/>
       <c r="B34" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="150" t="s">
+      <c r="C34" s="151" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="151"/>
-      <c r="E34" s="152"/>
-    </row>
-    <row r="35" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D34" s="152"/>
+      <c r="E34" s="153"/>
+    </row>
+    <row r="35" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="37"/>
       <c r="B35" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="150" t="s">
+      <c r="C35" s="151" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="151"/>
-      <c r="E35" s="152"/>
-    </row>
-    <row r="36" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D35" s="152"/>
+      <c r="E35" s="153"/>
+    </row>
+    <row r="36" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="37"/>
-      <c r="B36" s="176" t="s">
+      <c r="B36" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="177"/>
-      <c r="D36" s="177"/>
-      <c r="E36" s="178"/>
-    </row>
-    <row r="37" spans="1:7" ht="16.5" customHeight="1">
+      <c r="C36" s="162"/>
+      <c r="D36" s="162"/>
+      <c r="E36" s="163"/>
+    </row>
+    <row r="37" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="37"/>
       <c r="B37" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="150" t="s">
+      <c r="C37" s="151" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="151"/>
-      <c r="E37" s="152"/>
-    </row>
-    <row r="38" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D37" s="152"/>
+      <c r="E37" s="153"/>
+    </row>
+    <row r="38" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="37"/>
       <c r="B38" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="150" t="s">
+      <c r="C38" s="151" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="151"/>
-      <c r="E38" s="152"/>
-    </row>
-    <row r="39" spans="1:7" ht="17.25" customHeight="1">
+      <c r="D38" s="152"/>
+      <c r="E38" s="153"/>
+    </row>
+    <row r="39" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="37"/>
       <c r="B39" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="150" t="s">
+      <c r="C39" s="151" t="s">
         <v>102</v>
       </c>
-      <c r="D39" s="151"/>
-      <c r="E39" s="152"/>
-    </row>
-    <row r="40" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D39" s="152"/>
+      <c r="E39" s="153"/>
+    </row>
+    <row r="40" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="37"/>
       <c r="B40" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="C40" s="150" t="s">
+      <c r="C40" s="151" t="s">
         <v>145</v>
       </c>
-      <c r="D40" s="151"/>
-      <c r="E40" s="152"/>
-    </row>
-    <row r="41" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D40" s="152"/>
+      <c r="E40" s="153"/>
+    </row>
+    <row r="41" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="37"/>
       <c r="B41" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="150" t="s">
+      <c r="C41" s="151" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="151"/>
-      <c r="E41" s="152"/>
-    </row>
-    <row r="42" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D41" s="152"/>
+      <c r="E41" s="153"/>
+    </row>
+    <row r="42" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="37"/>
       <c r="B42" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="150" t="s">
+      <c r="C42" s="151" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="151"/>
-      <c r="E42" s="152"/>
-    </row>
-    <row r="43" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D42" s="152"/>
+      <c r="E42" s="153"/>
+    </row>
+    <row r="43" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="37"/>
       <c r="B43" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="150" t="s">
+      <c r="C43" s="151" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="151"/>
-      <c r="E43" s="152"/>
-    </row>
-    <row r="44" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D43" s="152"/>
+      <c r="E43" s="153"/>
+    </row>
+    <row r="44" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="37"/>
       <c r="B44" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="150" t="s">
+      <c r="C44" s="151" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="151"/>
-      <c r="E44" s="152"/>
-    </row>
-    <row r="45" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D44" s="152"/>
+      <c r="E44" s="153"/>
+    </row>
+    <row r="45" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="37"/>
       <c r="B45" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="150" t="s">
+      <c r="C45" s="151" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="151"/>
-      <c r="E45" s="152"/>
-    </row>
-    <row r="46" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D45" s="152"/>
+      <c r="E45" s="153"/>
+    </row>
+    <row r="46" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="37"/>
       <c r="B46" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="150" t="s">
+      <c r="C46" s="151" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="151"/>
-      <c r="E46" s="152"/>
-    </row>
-    <row r="47" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D46" s="152"/>
+      <c r="E46" s="153"/>
+    </row>
+    <row r="47" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="37"/>
       <c r="B47" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="150" t="s">
+      <c r="C47" s="151" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="151"/>
-      <c r="E47" s="152"/>
-    </row>
-    <row r="48" spans="1:7" ht="16.5" customHeight="1">
+      <c r="D47" s="152"/>
+      <c r="E47" s="153"/>
+    </row>
+    <row r="48" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="37"/>
       <c r="B48" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="150" t="s">
+      <c r="C48" s="151" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="151"/>
-      <c r="E48" s="152"/>
-    </row>
-    <row r="49" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D48" s="152"/>
+      <c r="E48" s="153"/>
+    </row>
+    <row r="49" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="37"/>
       <c r="B49" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="150" t="s">
+      <c r="C49" s="151" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="151"/>
-      <c r="E49" s="152"/>
-    </row>
-    <row r="50" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D49" s="152"/>
+      <c r="E49" s="153"/>
+    </row>
+    <row r="50" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="57"/>
       <c r="B50" s="88"/>
       <c r="C50" s="60"/>
@@ -5755,7 +5754,7 @@
       <c r="L50" s="57"/>
       <c r="M50" s="57"/>
     </row>
-    <row r="51" spans="1:13" s="57" customFormat="1" ht="16.5" customHeight="1">
+    <row r="51" spans="1:13" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="37"/>
       <c r="B51" s="50"/>
       <c r="C51" s="38"/>
@@ -5770,24 +5769,24 @@
       <c r="L51" s="38"/>
       <c r="M51" s="38"/>
     </row>
-    <row r="52" spans="1:13" s="57" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B52" s="156" t="s">
+    <row r="52" spans="1:13" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B52" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="157"/>
-      <c r="D52" s="157"/>
-      <c r="E52" s="158"/>
-    </row>
-    <row r="53" spans="1:13" ht="16.5" customHeight="1">
+      <c r="C52" s="165"/>
+      <c r="D52" s="165"/>
+      <c r="E52" s="166"/>
+    </row>
+    <row r="53" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="57"/>
       <c r="B53" s="140" t="s">
         <v>48</v>
       </c>
-      <c r="C53" s="159" t="s">
+      <c r="C53" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="160"/>
-      <c r="E53" s="161"/>
+      <c r="D53" s="168"/>
+      <c r="E53" s="169"/>
       <c r="F53" s="57"/>
       <c r="G53" s="57"/>
       <c r="H53" s="57"/>
@@ -5797,346 +5796,346 @@
       <c r="L53" s="57"/>
       <c r="M53" s="57"/>
     </row>
-    <row r="54" spans="1:13" ht="16.5" customHeight="1">
+    <row r="54" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="37"/>
       <c r="B54" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="C54" s="150" t="s">
+      <c r="C54" s="151" t="s">
         <v>75</v>
       </c>
-      <c r="D54" s="151"/>
-      <c r="E54" s="152"/>
-    </row>
-    <row r="55" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D54" s="152"/>
+      <c r="E54" s="153"/>
+    </row>
+    <row r="55" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="37"/>
       <c r="B55" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C55" s="150" t="s">
+      <c r="C55" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="151"/>
-      <c r="E55" s="152"/>
-    </row>
-    <row r="56" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D55" s="152"/>
+      <c r="E55" s="153"/>
+    </row>
+    <row r="56" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="37"/>
       <c r="B56" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="150" t="s">
+      <c r="C56" s="151" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="151"/>
-      <c r="E56" s="152"/>
-    </row>
-    <row r="57" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D56" s="152"/>
+      <c r="E56" s="153"/>
+    </row>
+    <row r="57" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="37"/>
       <c r="B57" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="150" t="s">
+      <c r="C57" s="151" t="s">
         <v>105</v>
       </c>
-      <c r="D57" s="154"/>
-      <c r="E57" s="155"/>
-    </row>
-    <row r="58" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D57" s="158"/>
+      <c r="E57" s="159"/>
+    </row>
+    <row r="58" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="37"/>
       <c r="B58" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="150" t="s">
+      <c r="C58" s="151" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="154"/>
-      <c r="E58" s="155"/>
-    </row>
-    <row r="59" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D58" s="158"/>
+      <c r="E58" s="159"/>
+    </row>
+    <row r="59" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="37"/>
       <c r="B59" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="150" t="s">
+      <c r="C59" s="151" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="154"/>
-      <c r="E59" s="155"/>
-    </row>
-    <row r="60" spans="1:13" ht="54" customHeight="1">
+      <c r="D59" s="158"/>
+      <c r="E59" s="159"/>
+    </row>
+    <row r="60" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="37"/>
       <c r="B60" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="150" t="s">
+      <c r="C60" s="151" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="154"/>
-      <c r="E60" s="155"/>
-    </row>
-    <row r="61" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D60" s="158"/>
+      <c r="E60" s="159"/>
+    </row>
+    <row r="61" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="37"/>
       <c r="B61" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="153" t="s">
+      <c r="C61" s="160" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="154"/>
-      <c r="E61" s="155"/>
-    </row>
-    <row r="62" spans="1:13" ht="30" customHeight="1">
+      <c r="D61" s="158"/>
+      <c r="E61" s="159"/>
+    </row>
+    <row r="62" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="37"/>
       <c r="B62" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="150" t="s">
+      <c r="C62" s="151" t="s">
         <v>56</v>
       </c>
-      <c r="D62" s="154"/>
-      <c r="E62" s="155"/>
-    </row>
-    <row r="63" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D62" s="158"/>
+      <c r="E62" s="159"/>
+    </row>
+    <row r="63" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="37"/>
       <c r="B63" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="153" t="s">
+      <c r="C63" s="160" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="154"/>
-      <c r="E63" s="155"/>
-    </row>
-    <row r="64" spans="1:13" ht="16.5" customHeight="1">
+      <c r="D63" s="158"/>
+      <c r="E63" s="159"/>
+    </row>
+    <row r="64" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="37"/>
       <c r="B64" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="153" t="s">
+      <c r="C64" s="160" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="154"/>
-      <c r="E64" s="155"/>
-    </row>
-    <row r="65" spans="1:8" ht="16.5" customHeight="1">
+      <c r="D64" s="158"/>
+      <c r="E64" s="159"/>
+    </row>
+    <row r="65" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="37"/>
       <c r="B65" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="150" t="s">
+      <c r="C65" s="151" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="151"/>
-      <c r="E65" s="152"/>
-    </row>
-    <row r="66" spans="1:8" ht="16.5" customHeight="1">
+      <c r="D65" s="152"/>
+      <c r="E65" s="153"/>
+    </row>
+    <row r="66" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="37"/>
       <c r="B66" s="46"/>
       <c r="C66" s="54"/>
       <c r="D66" s="55"/>
       <c r="E66" s="55"/>
     </row>
-    <row r="67" spans="1:8" ht="16.5" customHeight="1">
+    <row r="67" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="37"/>
-      <c r="B67" s="180"/>
-      <c r="C67" s="180"/>
-      <c r="D67" s="180"/>
-      <c r="E67" s="180"/>
+      <c r="B67" s="154"/>
+      <c r="C67" s="154"/>
+      <c r="D67" s="154"/>
+      <c r="E67" s="154"/>
       <c r="F67" s="56"/>
       <c r="G67" s="56"/>
       <c r="H67" s="56"/>
     </row>
-    <row r="68" spans="1:8" ht="16.5" customHeight="1">
+    <row r="68" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="37"/>
-      <c r="B68" s="179"/>
-      <c r="C68" s="179"/>
-      <c r="D68" s="179"/>
-      <c r="E68" s="179"/>
+      <c r="B68" s="150"/>
+      <c r="C68" s="150"/>
+      <c r="D68" s="150"/>
+      <c r="E68" s="150"/>
       <c r="F68" s="56"/>
       <c r="G68" s="56"/>
       <c r="H68" s="56"/>
     </row>
-    <row r="69" spans="1:8" ht="16.5" customHeight="1">
+    <row r="69" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="37"/>
-      <c r="B69" s="179"/>
-      <c r="C69" s="179"/>
-      <c r="D69" s="179"/>
-      <c r="E69" s="179"/>
+      <c r="B69" s="150"/>
+      <c r="C69" s="150"/>
+      <c r="D69" s="150"/>
+      <c r="E69" s="150"/>
       <c r="F69" s="56"/>
       <c r="G69" s="56"/>
       <c r="H69" s="56"/>
     </row>
-    <row r="70" spans="1:8" ht="16.5" customHeight="1">
+    <row r="70" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="37"/>
-      <c r="B70" s="179"/>
-      <c r="C70" s="179"/>
-      <c r="D70" s="179"/>
-      <c r="E70" s="179"/>
+      <c r="B70" s="150"/>
+      <c r="C70" s="150"/>
+      <c r="D70" s="150"/>
+      <c r="E70" s="150"/>
       <c r="F70" s="56"/>
       <c r="G70" s="56"/>
       <c r="H70" s="56"/>
     </row>
-    <row r="71" spans="1:8" ht="16.5" customHeight="1">
+    <row r="71" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="37"/>
-      <c r="B71" s="179"/>
-      <c r="C71" s="179"/>
-      <c r="D71" s="179"/>
-      <c r="E71" s="179"/>
+      <c r="B71" s="150"/>
+      <c r="C71" s="150"/>
+      <c r="D71" s="150"/>
+      <c r="E71" s="150"/>
       <c r="F71" s="56"/>
       <c r="G71" s="56"/>
       <c r="H71" s="56"/>
     </row>
-    <row r="72" spans="1:8" ht="16.5" customHeight="1">
+    <row r="72" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="37"/>
-      <c r="B72" s="179"/>
-      <c r="C72" s="179"/>
-      <c r="D72" s="179"/>
-      <c r="E72" s="179"/>
+      <c r="B72" s="150"/>
+      <c r="C72" s="150"/>
+      <c r="D72" s="150"/>
+      <c r="E72" s="150"/>
       <c r="F72" s="56"/>
       <c r="G72" s="56"/>
       <c r="H72" s="56"/>
     </row>
-    <row r="73" spans="1:8" ht="16.5" customHeight="1">
+    <row r="73" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="42"/>
-      <c r="B73" s="179"/>
-      <c r="C73" s="179"/>
-      <c r="D73" s="179"/>
-      <c r="E73" s="179"/>
+      <c r="B73" s="150"/>
+      <c r="C73" s="150"/>
+      <c r="D73" s="150"/>
+      <c r="E73" s="150"/>
       <c r="F73" s="56"/>
       <c r="G73" s="56"/>
       <c r="H73" s="56"/>
     </row>
-    <row r="74" spans="1:8" ht="16.5" customHeight="1">
+    <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="37"/>
-      <c r="B74" s="179"/>
-      <c r="C74" s="179"/>
-      <c r="D74" s="179"/>
-      <c r="E74" s="179"/>
+      <c r="B74" s="150"/>
+      <c r="C74" s="150"/>
+      <c r="D74" s="150"/>
+      <c r="E74" s="150"/>
       <c r="F74" s="56"/>
       <c r="G74" s="56"/>
       <c r="H74" s="56"/>
     </row>
-    <row r="75" spans="1:8" ht="16.5" customHeight="1">
+    <row r="75" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="37"/>
-      <c r="B75" s="179"/>
-      <c r="C75" s="179"/>
-      <c r="D75" s="179"/>
-      <c r="E75" s="179"/>
+      <c r="B75" s="150"/>
+      <c r="C75" s="150"/>
+      <c r="D75" s="150"/>
+      <c r="E75" s="150"/>
       <c r="F75" s="56"/>
       <c r="G75" s="56"/>
       <c r="H75" s="56"/>
     </row>
-    <row r="76" spans="1:8" ht="16.5" customHeight="1">
+    <row r="76" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="37"/>
-      <c r="B76" s="179"/>
-      <c r="C76" s="179"/>
-      <c r="D76" s="179"/>
-      <c r="E76" s="179"/>
+      <c r="B76" s="150"/>
+      <c r="C76" s="150"/>
+      <c r="D76" s="150"/>
+      <c r="E76" s="150"/>
       <c r="F76" s="56"/>
       <c r="G76" s="56"/>
       <c r="H76" s="56"/>
     </row>
-    <row r="77" spans="1:8" ht="16.5" customHeight="1">
+    <row r="77" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="37"/>
-      <c r="B77" s="179"/>
-      <c r="C77" s="179"/>
-      <c r="D77" s="179"/>
-      <c r="E77" s="179"/>
+      <c r="B77" s="150"/>
+      <c r="C77" s="150"/>
+      <c r="D77" s="150"/>
+      <c r="E77" s="150"/>
       <c r="F77" s="56"/>
       <c r="G77" s="56"/>
       <c r="H77" s="56"/>
     </row>
-    <row r="78" spans="1:8" ht="16.5" customHeight="1">
+    <row r="78" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="37"/>
-      <c r="B78" s="179"/>
-      <c r="C78" s="179"/>
-      <c r="D78" s="179"/>
-      <c r="E78" s="179"/>
+      <c r="B78" s="150"/>
+      <c r="C78" s="150"/>
+      <c r="D78" s="150"/>
+      <c r="E78" s="150"/>
       <c r="F78" s="56"/>
       <c r="G78" s="56"/>
       <c r="H78" s="56"/>
     </row>
-    <row r="79" spans="1:8" ht="16.5" customHeight="1">
+    <row r="79" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="42"/>
-      <c r="B79" s="179"/>
-      <c r="C79" s="179"/>
-      <c r="D79" s="179"/>
-      <c r="E79" s="179"/>
+      <c r="B79" s="150"/>
+      <c r="C79" s="150"/>
+      <c r="D79" s="150"/>
+      <c r="E79" s="150"/>
       <c r="F79" s="56"/>
       <c r="G79" s="56"/>
       <c r="H79" s="56"/>
     </row>
-    <row r="80" spans="1:8" ht="16.5" customHeight="1">
+    <row r="80" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="42"/>
-      <c r="B80" s="179"/>
-      <c r="C80" s="179"/>
-      <c r="D80" s="179"/>
-      <c r="E80" s="179"/>
+      <c r="B80" s="150"/>
+      <c r="C80" s="150"/>
+      <c r="D80" s="150"/>
+      <c r="E80" s="150"/>
       <c r="F80" s="56"/>
       <c r="G80" s="56"/>
       <c r="H80" s="56"/>
     </row>
-    <row r="81" spans="1:8" ht="16.5" customHeight="1">
+    <row r="81" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="42"/>
-      <c r="B81" s="179"/>
-      <c r="C81" s="179"/>
-      <c r="D81" s="179"/>
-      <c r="E81" s="179"/>
+      <c r="B81" s="150"/>
+      <c r="C81" s="150"/>
+      <c r="D81" s="150"/>
+      <c r="E81" s="150"/>
       <c r="F81" s="56"/>
       <c r="G81" s="56"/>
       <c r="H81" s="56"/>
     </row>
-    <row r="82" spans="1:8" ht="16.5" customHeight="1">
+    <row r="82" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="42"/>
-      <c r="B82" s="179"/>
-      <c r="C82" s="179"/>
-      <c r="D82" s="179"/>
-      <c r="E82" s="179"/>
+      <c r="B82" s="150"/>
+      <c r="C82" s="150"/>
+      <c r="D82" s="150"/>
+      <c r="E82" s="150"/>
       <c r="F82" s="56"/>
       <c r="G82" s="56"/>
       <c r="H82" s="56"/>
     </row>
-    <row r="83" spans="1:8" ht="16.5" customHeight="1">
+    <row r="83" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="42"/>
-      <c r="B83" s="179"/>
-      <c r="C83" s="179"/>
-      <c r="D83" s="179"/>
-      <c r="E83" s="179"/>
+      <c r="B83" s="150"/>
+      <c r="C83" s="150"/>
+      <c r="D83" s="150"/>
+      <c r="E83" s="150"/>
       <c r="F83" s="56"/>
       <c r="G83" s="56"/>
       <c r="H83" s="56"/>
     </row>
-    <row r="84" spans="1:8" ht="16.5" customHeight="1">
+    <row r="84" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="42"/>
-      <c r="B84" s="179"/>
-      <c r="C84" s="179"/>
-      <c r="D84" s="179"/>
-      <c r="E84" s="179"/>
+      <c r="B84" s="150"/>
+      <c r="C84" s="150"/>
+      <c r="D84" s="150"/>
+      <c r="E84" s="150"/>
       <c r="F84" s="56"/>
       <c r="G84" s="56"/>
       <c r="H84" s="56"/>
     </row>
-    <row r="85" spans="1:8" ht="16.5" customHeight="1">
+    <row r="85" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="42"/>
-      <c r="B85" s="179"/>
-      <c r="C85" s="179"/>
-      <c r="D85" s="179"/>
-      <c r="E85" s="179"/>
+      <c r="B85" s="150"/>
+      <c r="C85" s="150"/>
+      <c r="D85" s="150"/>
+      <c r="E85" s="150"/>
       <c r="F85" s="56"/>
       <c r="G85" s="56"/>
       <c r="H85" s="56"/>
     </row>
-    <row r="86" spans="1:8" ht="16.5" customHeight="1">
+    <row r="86" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="42"/>
-      <c r="B86" s="179"/>
-      <c r="C86" s="179"/>
-      <c r="D86" s="179"/>
-      <c r="E86" s="179"/>
+      <c r="B86" s="150"/>
+      <c r="C86" s="150"/>
+      <c r="D86" s="150"/>
+      <c r="E86" s="150"/>
       <c r="F86" s="56"/>
       <c r="G86" s="56"/>
       <c r="H86" s="56"/>
     </row>
-    <row r="87" spans="1:8" ht="16.5" customHeight="1">
+    <row r="87" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="42"/>
       <c r="F87" s="56"/>
       <c r="G87" s="56"/>
@@ -6144,27 +6143,36 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C60:E60"/>
@@ -6181,36 +6189,27 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B84:E84"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6222,96 +6221,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja2">
+  <sheetPr codeName="Hoja2" enableFormatConditionsCalculation="0">
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A3:Y38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="3"/>
-    <col min="3" max="3" width="16.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="16.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="11.42578125" style="3"/>
-    <col min="14" max="14" width="23.5703125" style="3" customWidth="1"/>
-    <col min="15" max="24" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="3.5" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="16.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="31.5" style="3" customWidth="1"/>
+    <col min="6" max="7" width="16.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="10.83203125" style="3"/>
+    <col min="14" max="14" width="23.5" style="3" customWidth="1"/>
+    <col min="15" max="24" width="10.83203125" style="3"/>
     <col min="25" max="25" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="11.42578125" style="3"/>
+    <col min="26" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:25" ht="18" customHeight="1">
-      <c r="B3" s="186" t="s">
+    <row r="3" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="184" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="186"/>
-      <c r="D3" s="186"/>
-      <c r="E3" s="186"/>
-      <c r="F3" s="186"/>
-      <c r="G3" s="186"/>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
-      <c r="J3" s="186"/>
-      <c r="K3" s="186"/>
-      <c r="L3" s="186"/>
-      <c r="M3" s="186"/>
-      <c r="N3" s="186"/>
-    </row>
-    <row r="4" spans="2:25" ht="11.25" customHeight="1">
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="184"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="184"/>
+    </row>
+    <row r="4" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="2:25" ht="15" customHeight="1"/>
-    <row r="6" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B6" s="181" t="s">
+    <row r="5" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="6" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="186" t="s">
         <v>165</v>
       </c>
-      <c r="C6" s="182"/>
-      <c r="D6" s="183" t="s">
+      <c r="C6" s="187"/>
+      <c r="D6" s="181" t="s">
         <v>166</v>
       </c>
-      <c r="E6" s="184"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
+      <c r="E6" s="182"/>
+      <c r="F6" s="183"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="185"/>
       <c r="Y6" s="3"/>
     </row>
-    <row r="7" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="181" t="s">
+    <row r="7" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="186" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="182"/>
-      <c r="D7" s="183" t="s">
+      <c r="C7" s="187"/>
+      <c r="D7" s="181" t="s">
         <v>168</v>
       </c>
-      <c r="E7" s="184"/>
-      <c r="F7" s="185"/>
+      <c r="E7" s="182"/>
+      <c r="F7" s="183"/>
       <c r="Y7" s="3"/>
     </row>
-    <row r="8" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="181" t="s">
+    <row r="8" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="186" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="182"/>
-      <c r="D8" s="183" t="s">
+      <c r="C8" s="187"/>
+      <c r="D8" s="181" t="s">
         <v>169</v>
       </c>
-      <c r="E8" s="184"/>
-      <c r="F8" s="185"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="183"/>
       <c r="Y8" s="3"/>
     </row>
-    <row r="9" spans="2:25" s="5" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B9" s="181" t="s">
+    <row r="9" spans="2:25" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="186" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="182"/>
+      <c r="C9" s="187"/>
       <c r="D9" s="106">
         <v>42996</v>
       </c>
@@ -6323,26 +6322,26 @@
       </c>
       <c r="Y9" s="3"/>
     </row>
-    <row r="10" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B10" s="181" t="s">
+    <row r="10" spans="2:25" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="186" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="182"/>
-      <c r="D10" s="183" t="s">
+      <c r="C10" s="187"/>
+      <c r="D10" s="181" t="s">
         <v>210</v>
       </c>
-      <c r="E10" s="184"/>
-      <c r="F10" s="185"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="183"/>
       <c r="Y10" s="3"/>
     </row>
-    <row r="11" spans="2:25" s="20" customFormat="1" ht="15" customHeight="1">
+    <row r="11" spans="2:25" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
       <c r="D11" s="22"/>
       <c r="E11" s="22"/>
       <c r="Y11" s="23"/>
     </row>
-    <row r="12" spans="2:25" ht="38.25">
+    <row r="12" spans="2:25" ht="39" x14ac:dyDescent="0.15">
       <c r="B12" s="6" t="s">
         <v>32</v>
       </c>
@@ -6383,7 +6382,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="24">
+    <row r="13" spans="2:25" ht="24" x14ac:dyDescent="0.15">
       <c r="B13" s="36">
         <v>1</v>
       </c>
@@ -6424,7 +6423,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="24">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B14" s="36">
         <v>2</v>
       </c>
@@ -6465,7 +6464,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="15" spans="2:25" ht="24">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B15" s="36">
         <v>3</v>
       </c>
@@ -6506,7 +6505,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="2:25" ht="24">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.15">
       <c r="B16" s="36">
         <v>4</v>
       </c>
@@ -6547,7 +6546,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="36">
+    <row r="17" spans="1:14" ht="24" x14ac:dyDescent="0.15">
       <c r="B17" s="36">
         <v>5</v>
       </c>
@@ -6588,7 +6587,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="24">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B18" s="36">
         <v>6</v>
       </c>
@@ -6629,7 +6628,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="24">
+    <row r="19" spans="1:14" ht="24" x14ac:dyDescent="0.15">
       <c r="B19" s="36">
         <v>7</v>
       </c>
@@ -6670,7 +6669,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="36">
+    <row r="20" spans="1:14" ht="24" x14ac:dyDescent="0.15">
       <c r="B20" s="36">
         <v>8</v>
       </c>
@@ -6711,7 +6710,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="24">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B21" s="36">
         <v>9</v>
       </c>
@@ -6752,7 +6751,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="25.5">
+    <row r="22" spans="1:14" ht="26" x14ac:dyDescent="0.15">
       <c r="B22" s="36">
         <v>10</v>
       </c>
@@ -6793,7 +6792,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="24">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B23" s="36">
         <v>11</v>
       </c>
@@ -6834,7 +6833,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="25.5">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B24" s="36">
         <v>12</v>
       </c>
@@ -6875,7 +6874,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="25.5">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B25" s="36">
         <v>13</v>
       </c>
@@ -6916,7 +6915,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="25.5">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A26" s="10"/>
       <c r="B26" s="36">
         <v>14</v>
@@ -6958,7 +6957,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="25.5">
+    <row r="27" spans="1:14" ht="26" x14ac:dyDescent="0.15">
       <c r="B27" s="36">
         <v>15</v>
       </c>
@@ -6999,7 +6998,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="24">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B28" s="36">
         <v>16</v>
       </c>
@@ -7040,7 +7039,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="25.5">
+    <row r="29" spans="1:14" ht="26" x14ac:dyDescent="0.15">
       <c r="B29" s="36">
         <v>17</v>
       </c>
@@ -7081,7 +7080,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="25.5">
+    <row r="30" spans="1:14" ht="26" x14ac:dyDescent="0.15">
       <c r="B30" s="36">
         <v>18</v>
       </c>
@@ -7122,7 +7121,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="25.5">
+    <row r="31" spans="1:14" ht="26" x14ac:dyDescent="0.15">
       <c r="B31" s="36">
         <v>19</v>
       </c>
@@ -7163,7 +7162,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
       <c r="B32" s="36"/>
       <c r="C32" s="100"/>
       <c r="D32" s="100"/>
@@ -7180,7 +7179,7 @@
       <c r="M32" s="103"/>
       <c r="N32" s="103"/>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B33" s="36"/>
       <c r="C33" s="100"/>
       <c r="D33" s="100"/>
@@ -7197,7 +7196,7 @@
       <c r="M33" s="103"/>
       <c r="N33" s="103"/>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B34" s="36"/>
       <c r="C34" s="100"/>
       <c r="D34" s="100"/>
@@ -7214,7 +7213,7 @@
       <c r="M34" s="103"/>
       <c r="N34" s="103"/>
     </row>
-    <row r="35" spans="2:14" ht="25.5">
+    <row r="35" spans="2:14" ht="26" x14ac:dyDescent="0.15">
       <c r="B35" s="36"/>
       <c r="C35" s="100"/>
       <c r="D35" s="100"/>
@@ -7231,7 +7230,7 @@
       <c r="M35" s="103"/>
       <c r="N35" s="103"/>
     </row>
-    <row r="36" spans="2:14" ht="24">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B36" s="36">
         <v>20</v>
       </c>
@@ -7272,7 +7271,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="2:14" ht="12.75" customHeight="1">
+    <row r="37" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="8"/>
       <c r="J37" s="104">
         <f>SUM(J13:J36)</f>
@@ -7286,24 +7285,24 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="38" spans="2:14">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.15">
       <c r="B38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D10:F10"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B3:N3"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D10:F10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
@@ -7325,7 +7324,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja4"/>
+  <sheetPr codeName="Hoja4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -7335,24 +7334,24 @@
       <selection pane="bottomRight" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="16" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" style="18" customWidth="1"/>
-    <col min="7" max="7" width="52.7109375" style="18" customWidth="1"/>
-    <col min="8" max="9" width="16.5703125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="19" customWidth="1"/>
-    <col min="11" max="11" width="31.7109375" style="19" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="52.6640625" style="18" customWidth="1"/>
+    <col min="8" max="9" width="16.5" style="19" customWidth="1"/>
+    <col min="10" max="10" width="19.83203125" style="19" customWidth="1"/>
+    <col min="11" max="11" width="31.6640625" style="19" hidden="1" customWidth="1"/>
     <col min="12" max="14" width="12" style="17" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" style="19" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="19"/>
+    <col min="15" max="15" width="13.6640625" style="19" customWidth="1"/>
+    <col min="16" max="16384" width="9.1640625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:15" s="29" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="188" t="s">
         <v>30</v>
       </c>
@@ -7370,7 +7369,7 @@
       <c r="M1" s="189"/>
       <c r="N1" s="190"/>
     </row>
-    <row r="2" spans="1:15" s="29" customFormat="1" ht="11.45" customHeight="1">
+    <row r="2" spans="1:15" s="29" customFormat="1" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="30"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
@@ -7385,13 +7384,13 @@
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
     </row>
-    <row r="3" spans="1:15" s="24" customFormat="1" ht="12.75" customHeight="1">
+    <row r="3" spans="1:15" s="24" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="32"/>
       <c r="B3" s="35"/>
       <c r="C3" s="32"/>
       <c r="M3" s="32"/>
     </row>
-    <row r="4" spans="1:15" s="28" customFormat="1" ht="60" customHeight="1">
+    <row r="4" spans="1:15" s="28" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="27" t="s">
         <v>25</v>
       </c>
@@ -7438,7 +7437,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="24">
+    <row r="5" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A5" s="108">
         <v>1</v>
       </c>
@@ -7488,7 +7487,7 @@
       </c>
       <c r="O5" s="131"/>
     </row>
-    <row r="6" spans="1:15" ht="24">
+    <row r="6" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A6" s="108">
         <v>2</v>
       </c>
@@ -7539,7 +7538,7 @@
       </c>
       <c r="O6" s="131"/>
     </row>
-    <row r="7" spans="1:15" ht="24">
+    <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A7" s="108">
         <v>3</v>
       </c>
@@ -7590,7 +7589,7 @@
       </c>
       <c r="O7" s="131"/>
     </row>
-    <row r="8" spans="1:15" ht="24">
+    <row r="8" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A8" s="108">
         <v>4</v>
       </c>
@@ -7641,7 +7640,7 @@
       </c>
       <c r="O8" s="131"/>
     </row>
-    <row r="9" spans="1:15" ht="24">
+    <row r="9" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A9" s="108">
         <v>5</v>
       </c>
@@ -7692,7 +7691,7 @@
       </c>
       <c r="O9" s="131"/>
     </row>
-    <row r="10" spans="1:15" ht="36">
+    <row r="10" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A10" s="108">
         <v>6</v>
       </c>
@@ -7743,7 +7742,7 @@
       </c>
       <c r="O10" s="131"/>
     </row>
-    <row r="11" spans="1:15" ht="24">
+    <row r="11" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A11" s="108">
         <v>7</v>
       </c>
@@ -7794,7 +7793,7 @@
       </c>
       <c r="O11" s="131"/>
     </row>
-    <row r="12" spans="1:15" ht="24">
+    <row r="12" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A12" s="108">
         <v>8</v>
       </c>
@@ -7845,7 +7844,7 @@
       </c>
       <c r="O12" s="131"/>
     </row>
-    <row r="13" spans="1:15" ht="24">
+    <row r="13" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A13" s="108">
         <v>9</v>
       </c>
@@ -7896,7 +7895,7 @@
       </c>
       <c r="O13" s="131"/>
     </row>
-    <row r="14" spans="1:15" ht="24">
+    <row r="14" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A14" s="108">
         <v>10</v>
       </c>
@@ -7947,7 +7946,7 @@
       </c>
       <c r="O14" s="131"/>
     </row>
-    <row r="15" spans="1:15" ht="24">
+    <row r="15" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A15" s="108">
         <v>11</v>
       </c>
@@ -7997,7 +7996,7 @@
       </c>
       <c r="O15" s="131"/>
     </row>
-    <row r="16" spans="1:15" ht="24">
+    <row r="16" spans="1:15" ht="24" x14ac:dyDescent="0.15">
       <c r="A16" s="108">
         <v>12</v>
       </c>
@@ -8047,7 +8046,7 @@
       </c>
       <c r="O16" s="131"/>
     </row>
-    <row r="17" spans="1:18" ht="24">
+    <row r="17" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A17" s="108">
         <v>13</v>
       </c>
@@ -8098,7 +8097,7 @@
       </c>
       <c r="O17" s="131"/>
     </row>
-    <row r="18" spans="1:18" ht="36">
+    <row r="18" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A18" s="108">
         <v>14</v>
       </c>
@@ -8147,7 +8146,7 @@
       </c>
       <c r="O18" s="131"/>
     </row>
-    <row r="19" spans="1:18" ht="36">
+    <row r="19" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A19" s="108">
         <v>15</v>
       </c>
@@ -8198,7 +8197,7 @@
       </c>
       <c r="O19" s="131"/>
     </row>
-    <row r="20" spans="1:18" ht="36">
+    <row r="20" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A20" s="108">
         <v>16</v>
       </c>
@@ -8247,7 +8246,7 @@
       </c>
       <c r="O20" s="131"/>
     </row>
-    <row r="21" spans="1:18" ht="48">
+    <row r="21" spans="1:18" ht="48" x14ac:dyDescent="0.15">
       <c r="A21" s="108">
         <v>17</v>
       </c>
@@ -8296,7 +8295,7 @@
       </c>
       <c r="O21" s="131"/>
     </row>
-    <row r="22" spans="1:18" ht="24">
+    <row r="22" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A22" s="108">
         <v>18</v>
       </c>
@@ -8347,7 +8346,7 @@
       </c>
       <c r="O22" s="131"/>
     </row>
-    <row r="23" spans="1:18" ht="36">
+    <row r="23" spans="1:18" ht="36" x14ac:dyDescent="0.15">
       <c r="A23" s="108">
         <v>19</v>
       </c>
@@ -8398,7 +8397,7 @@
       </c>
       <c r="O23" s="131"/>
     </row>
-    <row r="24" spans="1:18" ht="24">
+    <row r="24" spans="1:18" ht="24" x14ac:dyDescent="0.15">
       <c r="A24" s="108">
         <v>20</v>
       </c>
@@ -8449,7 +8448,7 @@
       </c>
       <c r="O24" s="131"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.15">
       <c r="P25" s="146"/>
       <c r="Q25" s="146"/>
       <c r="R25" s="146"/>
@@ -8480,126 +8479,126 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja5"/>
+  <sheetPr codeName="Hoja5" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:K61"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="2.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
+    <col min="1" max="2" width="2.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="6" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13"/>
-      <c r="C2" s="204" t="s">
+      <c r="C2" s="191" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="204"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="204"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="204"/>
-      <c r="I2" s="204"/>
-      <c r="J2" s="204"/>
-      <c r="K2" s="204"/>
-    </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="16.5" customHeight="1">
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="191"/>
+      <c r="G2" s="191"/>
+      <c r="H2" s="191"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="191"/>
+      <c r="K2" s="191"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14"/>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14"/>
-      <c r="C4" s="205" t="s">
+      <c r="C4" s="192" t="s">
         <v>112</v>
       </c>
-      <c r="D4" s="205"/>
-      <c r="E4" s="194" t="str">
+      <c r="D4" s="192"/>
+      <c r="E4" s="193" t="str">
         <f>IF(Planificación!D6&lt;&gt;"",Planificación!D6,"")</f>
         <v>Keyla Cusi</v>
       </c>
-      <c r="F4" s="195"/>
-      <c r="G4" s="195"/>
-      <c r="H4" s="195"/>
-      <c r="I4" s="196"/>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1">
+      <c r="F4" s="194"/>
+      <c r="G4" s="194"/>
+      <c r="H4" s="194"/>
+      <c r="I4" s="195"/>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="14"/>
-      <c r="C5" s="206" t="str">
+      <c r="C5" s="196" t="str">
         <f>Planificación!B7</f>
         <v>Analista de Calidad</v>
       </c>
-      <c r="D5" s="207"/>
-      <c r="E5" s="194" t="str">
+      <c r="D5" s="197"/>
+      <c r="E5" s="193" t="str">
         <f>IF(Planificación!D7&lt;&gt;"",Planificación!D7,"")</f>
         <v xml:space="preserve">Freddy Choquecota </v>
       </c>
-      <c r="F5" s="195"/>
-      <c r="G5" s="195"/>
-      <c r="H5" s="195"/>
-      <c r="I5" s="196"/>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1">
+      <c r="F5" s="194"/>
+      <c r="G5" s="194"/>
+      <c r="H5" s="194"/>
+      <c r="I5" s="195"/>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="14"/>
-      <c r="C6" s="192" t="s">
+      <c r="C6" s="199" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="193"/>
-      <c r="E6" s="194" t="str">
+      <c r="D6" s="200"/>
+      <c r="E6" s="193" t="str">
         <f>IF(Planificación!D8&lt;&gt;"",Planificación!D8,"")</f>
         <v>David Trujillo</v>
       </c>
-      <c r="F6" s="195"/>
-      <c r="G6" s="195"/>
-      <c r="H6" s="195"/>
-      <c r="I6" s="196"/>
-    </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="24" customHeight="1">
+      <c r="F6" s="194"/>
+      <c r="G6" s="194"/>
+      <c r="H6" s="194"/>
+      <c r="I6" s="195"/>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14"/>
-      <c r="C7" s="198" t="s">
+      <c r="C7" s="202" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="198"/>
-      <c r="E7" s="199">
+      <c r="D7" s="202"/>
+      <c r="E7" s="203">
         <f>IF(Planificación!D9&lt;&gt;"",Planificación!D9,"")</f>
         <v>42996</v>
       </c>
-      <c r="F7" s="200"/>
-      <c r="G7" s="201" t="s">
+      <c r="F7" s="204"/>
+      <c r="G7" s="205" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="202"/>
+      <c r="H7" s="206"/>
       <c r="I7" s="117">
         <f>IF(Planificación!F9&lt;&gt;"",Planificación!F9,"")</f>
         <v>43024</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1">
+    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="14"/>
-      <c r="C8" s="198" t="s">
+      <c r="C8" s="202" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="203"/>
-      <c r="E8" s="194" t="str">
+      <c r="D8" s="207"/>
+      <c r="E8" s="193" t="str">
         <f>IF(Planificación!D10&lt;&gt;"",Planificación!D10,"")</f>
         <v>Octubre</v>
       </c>
-      <c r="F8" s="195"/>
-      <c r="G8" s="195"/>
-      <c r="H8" s="195"/>
-      <c r="I8" s="196"/>
-    </row>
-    <row r="13" spans="1:11" ht="15">
-      <c r="C13" s="197" t="s">
+      <c r="F8" s="194"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="194"/>
+      <c r="I8" s="195"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="C13" s="201" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="197"/>
+      <c r="D13" s="201"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
@@ -8607,7 +8606,7 @@
       <c r="I13" s="15"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C14" s="120" t="s">
         <v>40</v>
       </c>
@@ -8616,7 +8615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14.25" customHeight="1">
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C15" s="120" t="s">
         <v>24</v>
       </c>
@@ -8625,7 +8624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="C16" s="120" t="s">
         <v>41</v>
       </c>
@@ -8634,7 +8633,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:5">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C17" s="120" t="s">
         <v>19</v>
       </c>
@@ -8643,7 +8642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:5">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C18" s="120" t="s">
         <v>20</v>
       </c>
@@ -8652,43 +8651,43 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:5">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C19" s="25"/>
       <c r="D19" s="26"/>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="3:5">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C20" s="133"/>
       <c r="D20" s="26"/>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="3:5">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C21" s="133"/>
       <c r="D21" s="26"/>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="3:5">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C22" s="133"/>
       <c r="D22" s="26"/>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="3:5">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C23" s="133"/>
       <c r="D23" s="26"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="3:5">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C24" s="133"/>
       <c r="D24" s="26"/>
       <c r="E24" s="12"/>
     </row>
-    <row r="26" spans="3:5" ht="15" customHeight="1">
-      <c r="C26" s="191" t="s">
+    <row r="26" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C26" s="198" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="191"/>
-    </row>
-    <row r="27" spans="3:5">
+      <c r="D26" s="198"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C27" s="34" t="s">
         <v>35</v>
       </c>
@@ -8696,7 +8695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="3:5">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C28" s="122" t="s">
         <v>149</v>
       </c>
@@ -8705,7 +8704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="3:5">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C29" s="122" t="s">
         <v>150</v>
       </c>
@@ -8714,7 +8713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:5">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C30" s="122" t="s">
         <v>151</v>
       </c>
@@ -8723,7 +8722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:5">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C31" s="122" t="s">
         <v>37</v>
       </c>
@@ -8732,7 +8731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:5">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.15">
       <c r="C32" s="122" t="s">
         <v>36</v>
       </c>
@@ -8741,7 +8740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:4">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C33" s="123" t="s">
         <v>16</v>
       </c>
@@ -8750,13 +8749,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="3:4" ht="15">
-      <c r="C39" s="191" t="s">
+    <row r="39" spans="3:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="C39" s="198" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="191"/>
-    </row>
-    <row r="40" spans="3:4">
+      <c r="D39" s="198"/>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C40" s="123" t="s">
         <v>108</v>
       </c>
@@ -8765,7 +8764,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="41" spans="3:4">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C41" s="123" t="s">
         <v>109</v>
       </c>
@@ -8774,7 +8773,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="42" spans="3:4">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C42" s="123" t="s">
         <v>16</v>
       </c>
@@ -8783,13 +8782,13 @@
         <v>-0.89999999999999858</v>
       </c>
     </row>
-    <row r="56" spans="3:4" ht="15">
-      <c r="C56" s="191" t="s">
+    <row r="56" spans="3:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="C56" s="198" t="s">
         <v>148</v>
       </c>
-      <c r="D56" s="191"/>
-    </row>
-    <row r="57" spans="3:4">
+      <c r="D56" s="198"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C57" s="34" t="s">
         <v>35</v>
       </c>
@@ -8797,7 +8796,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="3:4">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C58" s="126" t="s">
         <v>94</v>
       </c>
@@ -8806,7 +8805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="3:4">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C59" s="126" t="s">
         <v>96</v>
       </c>
@@ -8815,7 +8814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:4">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C60" s="126" t="s">
         <v>97</v>
       </c>
@@ -8824,7 +8823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:4">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C61" s="123" t="s">
         <v>16</v>
       </c>
@@ -8835,11 +8834,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C2:K2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:I5"/>
     <mergeCell ref="C56:D56"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:I6"/>
@@ -8851,6 +8845,11 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C2:K2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:I5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8867,29 +8866,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3"/>
+  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:K42"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="75" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.28515625" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5" customWidth="1"/>
+    <col min="3" max="3" width="4.5" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="125" t="s">
         <v>120</v>
       </c>
@@ -8912,7 +8911,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.5" thickBot="1">
+    <row r="3" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="135"/>
       <c r="B3" s="135"/>
       <c r="D3" s="126" t="s">
@@ -8931,7 +8930,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="209" t="s">
         <v>158</v>
       </c>
@@ -8952,7 +8951,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="210"/>
       <c r="B5" s="137" t="s">
         <v>153</v>
@@ -8971,7 +8970,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="210"/>
       <c r="B6" s="137" t="s">
         <v>154</v>
@@ -8985,7 +8984,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="210"/>
       <c r="B7" s="137" t="s">
         <v>155</v>
@@ -9001,7 +9000,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="210"/>
       <c r="B8" s="137" t="s">
         <v>156</v>
@@ -9015,7 +9014,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="210"/>
       <c r="B9" s="137" t="s">
         <v>157</v>
@@ -9025,7 +9024,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="210"/>
       <c r="B10" s="137" t="s">
         <v>188</v>
@@ -9036,7 +9035,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="210"/>
       <c r="B11" s="137"/>
       <c r="F11" s="132"/>
@@ -9045,7 +9044,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="12.75" customHeight="1" thickBot="1">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A12" s="211"/>
       <c r="B12" s="138"/>
       <c r="F12" s="132"/>
@@ -9054,13 +9053,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="J13" s="208"/>
       <c r="K13" s="139" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="J14" s="208" t="s">
         <v>115</v>
       </c>
@@ -9068,61 +9067,61 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="J15" s="208"/>
       <c r="K15" s="139" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="J16" s="208"/>
       <c r="K16" s="139" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="17" spans="10:11">
+    <row r="17" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J17" s="208"/>
       <c r="K17" s="139" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="10:11">
+    <row r="18" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J18" s="208"/>
       <c r="K18" s="139" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="10:11">
+    <row r="19" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J19" s="208"/>
       <c r="K19" s="139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="10:11">
+    <row r="20" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J20" s="208"/>
       <c r="K20" s="139" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="10:11">
+    <row r="21" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J21" s="208"/>
       <c r="K21" s="139" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="10:11">
+    <row r="22" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J22" s="208"/>
       <c r="K22" s="139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="10:11">
+    <row r="23" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J23" s="208"/>
       <c r="K23" s="139" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="10:11">
+    <row r="24" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J24" s="208" t="s">
         <v>116</v>
       </c>
@@ -9130,43 +9129,43 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="10:11">
+    <row r="25" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J25" s="208"/>
       <c r="K25" s="139" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="10:11">
+    <row r="26" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J26" s="208"/>
       <c r="K26" s="139" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="10:11">
+    <row r="27" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J27" s="208"/>
       <c r="K27" s="139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="28" spans="10:11">
+    <row r="28" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J28" s="208"/>
       <c r="K28" s="139" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="10:11">
+    <row r="29" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J29" s="208"/>
       <c r="K29" s="139" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="10:11">
+    <row r="30" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J30" s="208"/>
       <c r="K30" s="139" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="10:11">
+    <row r="31" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J31" s="208" t="s">
         <v>117</v>
       </c>
@@ -9174,31 +9173,31 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="10:11">
+    <row r="32" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J32" s="208"/>
       <c r="K32" s="139" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="10:11">
+    <row r="33" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J33" s="208"/>
       <c r="K33" s="139" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="10:11">
+    <row r="34" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J34" s="208"/>
       <c r="K34" s="139" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="10:11">
+    <row r="35" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J35" s="208"/>
       <c r="K35" s="139" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="36" spans="10:11">
+    <row r="36" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J36" s="208" t="s">
         <v>118</v>
       </c>
@@ -9206,37 +9205,37 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="10:11">
+    <row r="37" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J37" s="208"/>
       <c r="K37" s="139" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="10:11">
+    <row r="38" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J38" s="208"/>
       <c r="K38" s="139" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="10:11">
+    <row r="39" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J39" s="208"/>
       <c r="K39" s="139" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="10:11">
+    <row r="40" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J40" s="208"/>
       <c r="K40" s="139" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="41" spans="10:11">
+    <row r="41" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J41" s="208"/>
       <c r="K41" s="139" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="42" spans="10:11">
+    <row r="42" spans="10:11" x14ac:dyDescent="0.15">
       <c r="J42" s="208"/>
       <c r="K42" s="139" t="s">
         <v>127</v>

</xml_diff>